<commit_message>
Changes specific to Education reports.
</commit_message>
<xml_diff>
--- a/Input File/Education/200809datasamplereport/EdnOnePageReports2008-09Data.xlsx
+++ b/Input File/Education/200809datasamplereport/EdnOnePageReports2008-09Data.xlsx
@@ -781,18 +781,9 @@
     <t>Pupil Teacher Ratio Private</t>
   </si>
   <si>
-    <t xml:space="preserve">Avg. % of SC/ST children in Class 1 </t>
-  </si>
-  <si>
-    <t>Avg. % of SC/ST children in Class 1 Private</t>
-  </si>
-  <si>
     <t>% Children Enrolled in Class 5 w.r.t. Class 1</t>
   </si>
   <si>
-    <t xml:space="preserve">% Schools with Toilets for Girls </t>
-  </si>
-  <si>
     <t>% Schools with Toilets for Girls Private</t>
   </si>
   <si>
@@ -800,9 +791,6 @@
   </si>
   <si>
     <t>% Children Enrolled in Class 5 w.r.t. Class 1 Govt.</t>
-  </si>
-  <si>
-    <t>Avg. % of SC/ST children in Class 1 Govt.</t>
   </si>
   <si>
     <t>Number of Schools Govt.</t>
@@ -821,10 +809,22 @@
     <t>Grant received per Child</t>
   </si>
   <si>
-    <t>% Schools with Water Facility  Private</t>
-  </si>
-  <si>
-    <t>% Schools with Water Facility  Govt.</t>
+    <t>Avg. % SC/ST children in Class 1 Private</t>
+  </si>
+  <si>
+    <t>Avg. % SC/ST children in Class 1 Govt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avg. % SC/ST children in Class 1 </t>
+  </si>
+  <si>
+    <t>% Schools with Toilets for Girls</t>
+  </si>
+  <si>
+    <t>% Schools with Water Facility Govt.</t>
+  </si>
+  <si>
+    <t>% Schools with Water Facility Private</t>
   </si>
 </sst>
 </file>
@@ -2512,13 +2512,13 @@
         <v>246</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>248</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>249</v>
@@ -2533,46 +2533,46 @@
         <v>252</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="O1" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>224</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="R1" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="S1" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>262</v>
-      </c>
       <c r="U1" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="V1" s="4" t="s">
-        <v>266</v>
-      </c>
       <c r="W1" s="4" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixes for minor issues and a couple of new options - year field in UI and checkbox for printing only one report (so that you can click back, uncheck this and then print all reports if first report is fine).
</commit_message>
<xml_diff>
--- a/Input File/Education/200809datasamplereport/EdnOnePageReports2008-09Data.xlsx
+++ b/Input File/Education/200809datasamplereport/EdnOnePageReports2008-09Data.xlsx
@@ -868,7 +868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -881,6 +881,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2479,9 +2482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2576,10 +2577,10 @@
       </c>
     </row>
     <row r="2" spans="1:24" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>247</v>
       </c>
       <c r="C2">

</xml_diff>